<commit_message>
:bug: fix: adição de mais uma query nos gráficos
</commit_message>
<xml_diff>
--- a/Graficos/gráficos.xlsx
+++ b/Graficos/gráficos.xlsx
@@ -1,33 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruna\Desktop\Resilia\Projetos\lego database\Gráficos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruna\Desktop\Resilia\Projetos\lego database\Graficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58D01644-867F-48BF-8424-7EB5D7316C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303319DB-493F-4A9A-920C-3AF3B25BBCBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="4560" yWindow="2880" windowWidth="13035" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUERY 1" sheetId="1" r:id="rId1"/>
-    <sheet name="QUERY 2" sheetId="2" r:id="rId2"/>
+    <sheet name="QUERY 2" sheetId="5" r:id="rId2"/>
     <sheet name="QUERY 3" sheetId="3" r:id="rId3"/>
     <sheet name="QUERY 4" sheetId="4" r:id="rId4"/>
+    <sheet name="QUERY 7" sheetId="2" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>ano</t>
   </si>
@@ -73,11 +74,47 @@
   <si>
     <t>Nexo Knights</t>
   </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Light Bluish Gray</t>
+  </si>
+  <si>
+    <t>Dark Bluish Gray</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Tan</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Light Gray</t>
+  </si>
+  <si>
+    <t>Reddish Brown</t>
+  </si>
+  <si>
+    <t>Trans-Clear</t>
+  </si>
+  <si>
+    <t>nome da cor</t>
+  </si>
+  <si>
+    <t>quantidade de peças</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1343,6 +1380,1691 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Cores</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> mais feitas de peças</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.7537513434722247E-2"/>
+          <c:y val="0.12056587091069851"/>
+          <c:w val="0.89668627098238374"/>
+          <c:h val="0.64533205232635049"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-163A-487B-B55B-FDB89A3846D4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-163A-487B-B55B-FDB89A3846D4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-163A-487B-B55B-FDB89A3846D4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-163A-487B-B55B-FDB89A3846D4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-163A-487B-B55B-FDB89A3846D4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-163A-487B-B55B-FDB89A3846D4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-163A-487B-B55B-FDB89A3846D4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-163A-487B-B55B-FDB89A3846D4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-163A-487B-B55B-FDB89A3846D4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-163A-487B-B55B-FDB89A3846D4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'QUERY 2'!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>White</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Light Bluish Gray</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dark Bluish Gray</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Yellow</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Tan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Red</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Blue</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Light Gray</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Reddish Brown</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Trans-Clear</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'QUERY 2'!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7282</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3454</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2672</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2320</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2137</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1351</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1136</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>788</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-163A-487B-B55B-FDB89A3846D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1519908448"/>
+        <c:axId val="1519890144"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1519908448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1519890144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1519890144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1519908448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>temas</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> mais repetidos (mais populares)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19525000000000001"/>
+          <c:y val="3.2407407407407406E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[2]supabase_osxkxnruvugmcquspame_N!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vezes repetido</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-828D-4460-BA5E-93808DDA2166}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-828D-4460-BA5E-93808DDA2166}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-828D-4460-BA5E-93808DDA2166}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-828D-4460-BA5E-93808DDA2166}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-828D-4460-BA5E-93808DDA2166}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-828D-4460-BA5E-93808DDA2166}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-828D-4460-BA5E-93808DDA2166}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-828D-4460-BA5E-93808DDA2166}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-828D-4460-BA5E-93808DDA2166}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>[2]supabase_osxkxnruvugmcquspame_N!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>371</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>494</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>435</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>443</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>453</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[2]supabase_osxkxnruvugmcquspame_N!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000012-828D-4460-BA5E-93808DDA2166}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1448583919"/>
+        <c:axId val="1448582671"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1448583919"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1448582671"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1448582671"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1448583919"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>T</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t>emas mais populares nos 10 anos que mais sets foram criados</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F8FB-410A-896B-AEF3D9D63D15}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-F8FB-410A-896B-AEF3D9D63D15}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-F8FB-410A-896B-AEF3D9D63D15}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-F8FB-410A-896B-AEF3D9D63D15}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-F8FB-410A-896B-AEF3D9D63D15}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-64C0-47F5-B9F0-A29AA65C97A0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-F8FB-410A-896B-AEF3D9D63D15}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-F8FB-410A-896B-AEF3D9D63D15}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-F8FB-410A-896B-AEF3D9D63D15}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-F8FB-410A-896B-AEF3D9D63D15}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:effectLst>
+                      <a:glow rad="127000">
+                        <a:schemeClr val="tx1"/>
+                      </a:glow>
+                    </a:effectLst>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'QUERY 4'!$C$2:$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Technic</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Basketball</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>City</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>City</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Ninjago</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ninjago</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Duplo</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Gear</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Friends</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Nexo Knights</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'QUERY 4'!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F8FB-410A-896B-AEF3D9D63D15}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>anos</a:t>
             </a:r>
@@ -2185,1087 +3907,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>temas</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> mais repetidos (mais populares)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.19525000000000001"/>
-          <c:y val="3.2407407407407406E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[2]supabase_osxkxnruvugmcquspame_N!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>vezes repetido</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="C00000"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-828D-4460-BA5E-93808DDA2166}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-828D-4460-BA5E-93808DDA2166}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-828D-4460-BA5E-93808DDA2166}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="92D050"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-828D-4460-BA5E-93808DDA2166}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-828D-4460-BA5E-93808DDA2166}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-828D-4460-BA5E-93808DDA2166}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000D-828D-4460-BA5E-93808DDA2166}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000F-828D-4460-BA5E-93808DDA2166}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000011-828D-4460-BA5E-93808DDA2166}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>[2]supabase_osxkxnruvugmcquspame_N!$A$2:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>501</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>371</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>504</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>494</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>435</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>443</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>453</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[2]supabase_osxkxnruvugmcquspame_N!$B$2:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>246</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>219</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>192</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>191</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>185</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>172</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000012-828D-4460-BA5E-93808DDA2166}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1448583919"/>
-        <c:axId val="1448582671"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1448583919"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1448582671"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1448582671"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1448583919"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pt-BR"/>
-              <a:t>T</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" baseline="0"/>
-              <a:t>emas mais populares nos 10 anos que mais sets foram criados</a:t>
-            </a:r>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-F8FB-410A-896B-AEF3D9D63D15}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-F8FB-410A-896B-AEF3D9D63D15}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000008-F8FB-410A-896B-AEF3D9D63D15}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-F8FB-410A-896B-AEF3D9D63D15}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-F8FB-410A-896B-AEF3D9D63D15}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="92D050"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-F8FB-410A-896B-AEF3D9D63D15}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000004-F8FB-410A-896B-AEF3D9D63D15}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-F8FB-410A-896B-AEF3D9D63D15}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000002-F8FB-410A-896B-AEF3D9D63D15}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1"/>
-                    </a:solidFill>
-                    <a:effectLst>
-                      <a:glow rad="127000">
-                        <a:schemeClr val="tx1"/>
-                      </a:glow>
-                    </a:effectLst>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:round/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'QUERY 4'!$C$2:$C$11</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Technic</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Basketball</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>City</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>City</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Ninjago</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Ninjago</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Duplo</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Gear</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Friends</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Nexo Knights</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'QUERY 4'!$D$2:$D$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>51</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F8FB-410A-896B-AEF3D9D63D15}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3426,6 +4067,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -5424,6 +6105,509 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5504,26 +6688,24 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2">
+        <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43C03870-4B55-43F4-A0B6-6DCF9F72A315}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9054417A-43B0-074C-718D-605A2FFE50D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -5608,6 +6790,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43C03870-4B55-43F4-A0B6-6DCF9F72A315}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6206,10 +7431,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -6317,189 +7542,105 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F4A2735-4465-4F76-B63E-E2C231397C39}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1975</v>
+      <c r="A2" t="s">
+        <v>15</v>
       </c>
       <c r="B2">
-        <v>31</v>
+        <v>7282</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1974</v>
+      <c r="A3" t="s">
+        <v>16</v>
       </c>
       <c r="B3">
-        <v>39</v>
+        <v>3454</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1972</v>
+      <c r="A4" t="s">
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>38</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1971</v>
+      <c r="A5" t="s">
+        <v>18</v>
       </c>
       <c r="B5">
-        <v>45</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1970</v>
+      <c r="A6" t="s">
+        <v>19</v>
       </c>
       <c r="B6">
-        <v>29</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1968</v>
+      <c r="A7" t="s">
+        <v>20</v>
       </c>
       <c r="B7">
-        <v>25</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1967</v>
+      <c r="A8" t="s">
+        <v>21</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1965</v>
+      <c r="A9" t="s">
+        <v>22</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1964</v>
+      <c r="A10" t="s">
+        <v>23</v>
       </c>
       <c r="B10">
-        <v>11</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1963</v>
+      <c r="A11" t="s">
+        <v>24</v>
       </c>
       <c r="B11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1962</v>
-      </c>
-      <c r="B12">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1961</v>
-      </c>
-      <c r="B13">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1960</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1959</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1958</v>
-      </c>
-      <c r="B16">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1957</v>
-      </c>
-      <c r="B17">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1956</v>
-      </c>
-      <c r="B18">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1955</v>
-      </c>
-      <c r="B19">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1954</v>
-      </c>
-      <c r="B20">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1953</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1950</v>
-      </c>
-      <c r="B22">
-        <v>7</v>
+        <v>788</v>
       </c>
     </row>
   </sheetData>
@@ -6509,7 +7650,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6613,7 +7754,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6784,4 +7925,196 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N24" sqref="C24:N25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1975</v>
+      </c>
+      <c r="B2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1974</v>
+      </c>
+      <c r="B3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1972</v>
+      </c>
+      <c r="B4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1971</v>
+      </c>
+      <c r="B5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1970</v>
+      </c>
+      <c r="B6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1968</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1967</v>
+      </c>
+      <c r="B8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1965</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1964</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1963</v>
+      </c>
+      <c r="B11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1962</v>
+      </c>
+      <c r="B12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1961</v>
+      </c>
+      <c r="B13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1960</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1959</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1958</v>
+      </c>
+      <c r="B16">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1957</v>
+      </c>
+      <c r="B17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1956</v>
+      </c>
+      <c r="B18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1955</v>
+      </c>
+      <c r="B19">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1954</v>
+      </c>
+      <c r="B20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1953</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1950</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>